<commit_message>
change a var name
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14214\Documents\MATLAB\Util\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB9D2A3-0120-48C3-AF6E-BD7D4AF73076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2A2F58-F0EF-46A8-90E3-E7170A3D39E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,11 +35,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>R^2</t>
+    <t>编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>编号</t>
+    <t>testRSS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,7 +368,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -380,7 +380,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -389,7 +389,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>